<commit_message>
mejorado diccionario de datos
</commit_message>
<xml_diff>
--- a/sql/Diccionario de datos proyecto final.xlsx
+++ b/sql/Diccionario de datos proyecto final.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CBA9432-73D4-473D-BC76-6895B001FE75}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex-Pc\Documents\GitHub\proyecto-final\sql\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D8190C-D894-43C4-BF54-80180ED588CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="employees" sheetId="1" r:id="rId1"/>
+    <sheet name="cafe_users" sheetId="2" r:id="rId2"/>
+    <sheet name="orders" sheetId="3" r:id="rId3"/>
+    <sheet name="orders_employees" sheetId="4" r:id="rId4"/>
+    <sheet name="shops" sheetId="5" r:id="rId5"/>
+    <sheet name="shop_products" sheetId="6" r:id="rId6"/>
+    <sheet name="orders_details" sheetId="7" r:id="rId7"/>
+    <sheet name="products" sheetId="8" r:id="rId8"/>
+    <sheet name="categories" sheetId="9" r:id="rId9"/>
+    <sheet name="sessions" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="118">
   <si>
     <t>Campo</t>
   </si>
@@ -243,80 +244,152 @@
     <t>Telefono de la tienda</t>
   </si>
   <si>
-    <t>Email de la tienda</t>
-  </si>
-  <si>
-    <t>Tabla: shop_products</t>
-  </si>
-  <si>
-    <t>product_id</t>
-  </si>
-  <si>
     <t>NUMBER</t>
   </si>
   <si>
-    <t>Identificador unico de los productos</t>
-  </si>
-  <si>
-    <t>Tabla: order_details</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>Cantidad de productos</t>
-  </si>
-  <si>
-    <t>Tabla: products</t>
-  </si>
-  <si>
-    <t>products_id</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>Nombre del producto</t>
-  </si>
-  <si>
-    <t>product_description</t>
-  </si>
-  <si>
-    <t>varchar2(200)</t>
-  </si>
-  <si>
-    <t>Descripcion del producto</t>
-  </si>
-  <si>
-    <t>stock</t>
-  </si>
-  <si>
-    <t>Stock del producto</t>
-  </si>
-  <si>
-    <t>reviews</t>
-  </si>
-  <si>
-    <t>Reviews del producto</t>
-  </si>
-  <si>
-    <t>category_id</t>
-  </si>
-  <si>
-    <t>Identificador unico de la categoria</t>
-  </si>
-  <si>
-    <t>category_name</t>
-  </si>
-  <si>
-    <t>Nombre de la categoria</t>
+    <t>Columna</t>
+  </si>
+  <si>
+    <t>Tipo de datos</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_ID</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_NAME</t>
+  </si>
+  <si>
+    <t>VARCHAR2(30)</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_SURNAME</t>
+  </si>
+  <si>
+    <t>VARCHAR2(100)</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>POSITION</t>
+  </si>
+  <si>
+    <t>HIRE_DATE</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>USER_ID</t>
+  </si>
+  <si>
+    <t>USER_NAME</t>
+  </si>
+  <si>
+    <t>USER_SURNAME</t>
+  </si>
+  <si>
+    <t>VARCHAR2(50)</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>LAST_CONNECTION</t>
+  </si>
+  <si>
+    <t>ORDERS_ID</t>
+  </si>
+  <si>
+    <t>SHOP_ID</t>
+  </si>
+  <si>
+    <t>ORDER_DATE</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>ORDER_NAME</t>
+  </si>
+  <si>
+    <t>ORDER_SURNAME</t>
+  </si>
+  <si>
+    <t>TOTAL_PRICE</t>
+  </si>
+  <si>
+    <t>ORDER_STATE</t>
+  </si>
+  <si>
+    <t>SHOP_NAME</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>PRODUCT_ID</t>
+  </si>
+  <si>
+    <t>ORDER_DETAILS_ID</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>PRODUCTS_ID</t>
+  </si>
+  <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>PRODUCT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>VARCHAR2(200)</t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>REVIEWS</t>
+  </si>
+  <si>
+    <t>CATEGORY_ID</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>FLOAT(126)</t>
+  </si>
+  <si>
+    <t>IMAGE_URL</t>
+  </si>
+  <si>
+    <t>VARCHAR2(300)</t>
+  </si>
+  <si>
+    <t>CATEGORY_NAME</t>
+  </si>
+  <si>
+    <t>TOKEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +411,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,7 +436,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -407,17 +496,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD9D9E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9E3"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9E3"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +590,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -732,13 +886,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
@@ -746,7 +900,7 @@
     <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -774,7 +928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -786,7 +940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -798,7 +952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -810,7 +964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -822,7 +976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -834,7 +988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -846,7 +1000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -858,7 +1012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -870,12 +1024,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -900,7 +1054,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -912,7 +1066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -924,7 +1078,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -936,7 +1090,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -948,7 +1102,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
@@ -960,7 +1114,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -972,7 +1126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
@@ -984,12 +1138,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
@@ -1012,7 +1166,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -1024,15 +1178,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
@@ -1057,7 +1211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
@@ -1069,7 +1223,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>52</v>
       </c>
@@ -1081,7 +1235,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>54</v>
       </c>
@@ -1093,7 +1247,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>56</v>
       </c>
@@ -1105,7 +1259,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>58</v>
       </c>
@@ -1117,7 +1271,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>61</v>
       </c>
@@ -1129,12 +1283,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1157,7 +1311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
@@ -1169,12 +1323,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>52</v>
       </c>
@@ -1199,7 +1353,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>65</v>
       </c>
@@ -1211,7 +1365,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>67</v>
       </c>
@@ -1223,7 +1377,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>56</v>
       </c>
@@ -1235,7 +1389,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
@@ -1247,223 +1401,862 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" t="s">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="3" t="s">
+      <c r="C48" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="10"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F9C36B-6F78-4AEE-AC0A-D65995C40DAF}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="4" t="s">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A450008C-642A-4136-9FDA-F14EBF40CB7D}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D808D87-2204-4CD3-A6A7-DB4C182C8EED}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CBCB90-6872-4F3A-96A0-891C35FA386A}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501F6F75-A9A0-4220-90D7-3F49C4F5825E}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFCDF0C-3E48-4BB0-A753-4F50B3FBCF86}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FFBFBF-AAB6-4491-A6A6-3D46E86D01BE}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F13204-6444-4A26-906B-0BFF449B63CD}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51698A96-74D4-485D-B430-0663E2398DDE}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" s="5"/>
-      <c r="D59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>92</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" t="s">
-        <v>93</v>
-      </c>
+      <c r="C4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>